<commit_message>
ecobat site changes eg proforma
</commit_message>
<xml_diff>
--- a/Ecobat_ProForma_PN.xlsx
+++ b/Ecobat_ProForma_PN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\smbhome.uscs.susx.ac.uk\brs28\Desktop\MammalSociety\Ecobat\Ecobat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Personal\Beth\MammalSociety\Ecobat\Ecobat\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -65,8 +65,7 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>Please include site name for reference. Likely to be the same for all rows.
-This helps us to reference your location with a place name.</t>
+          <t>Please include a name for the location of each detector. For example, if you have 5 detectors in use, consider called them D1, D2, D3, D4, D5</t>
         </r>
       </text>
     </comment>
@@ -109,7 +108,8 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>Always specify in the order of LAT then LON. Thank you.</t>
+          <t>Always specify in the order of LAT then LON. Thank you.
+You will be asked to map this separately in the first step of the upload.</t>
         </r>
       </text>
     </comment>
@@ -135,7 +135,8 @@
             <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
-If using multiple spatial referencing systems, please define here e.g. British National Grid, OSGB, Latitude and Longitude.</t>
+If using multiple spatial referencing systems, please define here e.g. British National Grid, OSGB, Latitude and Longitude.
+You will be asked to map this separately in the first step of the upload.</t>
         </r>
       </text>
     </comment>
@@ -681,17 +682,6 @@
             <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
-This column is only required if your file has a mixture of privacy settings (otherwise sensitivity can be set when uploading on the Ecobat website)</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">. 
 </t>
         </r>
         <r>
@@ -716,7 +706,19 @@
           <t xml:space="preserve">
 Public
 Blur records to 10km grid square 
-Do not publish</t>
+Do not publish
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>You will also set this separately during the first step of the upload</t>
         </r>
       </text>
     </comment>
@@ -865,7 +867,18 @@
             <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">: Species presence within a 15 second sound file
- </t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>You will also set this separately during the first step of the upload</t>
         </r>
       </text>
     </comment>
@@ -1794,53 +1807,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="88">
   <si>
     <t>Sensitivity</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Species</t>
   </si>
   <si>
     <t>Detector Make</t>
   </si>
   <si>
-    <t>Detector Model</t>
-  </si>
-  <si>
-    <t>Detector height</t>
-  </si>
-  <si>
-    <t>Within 25m of known roost</t>
-  </si>
-  <si>
-    <t>Activity elevated as known roost nearby</t>
-  </si>
-  <si>
     <t>Detector next to linear feature</t>
   </si>
   <si>
-    <t>Detector &lt;25m of linear feature</t>
-  </si>
-  <si>
     <t>Detector next to anthropogenic feature</t>
   </si>
   <si>
-    <t>Detector &lt;25m of anthropogenic feature</t>
-  </si>
-  <si>
-    <t>Sunset Temperature (°C)</t>
-  </si>
-  <si>
     <t>Rainfall</t>
   </si>
   <si>
-    <t>Sunset Wind speed (mph)</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -1976,9 +1962,6 @@
     <t>Pass Definition</t>
   </si>
   <si>
-    <t>Site Name</t>
-  </si>
-  <si>
     <t>Pass 0.5s gap</t>
   </si>
   <si>
@@ -2048,10 +2031,46 @@
     <t>Passes per night</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>Spatial Reference System</t>
+  </si>
+  <si>
+    <t>Bat detector model</t>
+  </si>
+  <si>
+    <t>Bat detector make</t>
+  </si>
+  <si>
+    <t>Location of bat detector (geographic coordinates)</t>
+  </si>
+  <si>
+    <t>Date of bat survey</t>
+  </si>
+  <si>
+    <t>Height of bat detector (m)</t>
+  </si>
+  <si>
+    <t>Was the detector within 25m of known roost</t>
+  </si>
+  <si>
+    <t>Detector located &lt;25m of linear feature</t>
+  </si>
+  <si>
+    <t>Detector located &lt;25m of anthropogenic feature</t>
+  </si>
+  <si>
+    <t>Rainfall at sunset</t>
+  </si>
+  <si>
+    <t>Sunset temperature (C)</t>
+  </si>
+  <si>
+    <t>Sunset wind speed (mph)</t>
+  </si>
+  <si>
+    <t>Location name</t>
+  </si>
+  <si>
+    <t>Activity elevated as known bat roost nearby</t>
   </si>
 </sst>
 </file>
@@ -2304,7 +2323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2326,9 +2345,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2337,15 +2353,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2372,14 +2379,29 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2670,301 +2692,302 @@
   <dimension ref="A1:AG257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="16" style="15" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="16" style="14" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="19" customWidth="1"/>
-    <col min="7" max="7" width="10" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="15" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="15" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="19"/>
-    <col min="12" max="12" width="13.42578125" style="15" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" style="15" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="15"/>
-    <col min="16" max="16" width="13.5703125" style="15" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" style="15" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" style="19" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="15"/>
-    <col min="20" max="20" width="11.5703125" style="19" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" style="15" customWidth="1"/>
-    <col min="22" max="25" width="9.140625" style="15"/>
+    <col min="5" max="5" width="25" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="15" customWidth="1"/>
+    <col min="7" max="7" width="10" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="14" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="15"/>
+    <col min="12" max="12" width="13.42578125" style="14" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="14" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" style="14" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="14" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" style="14" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" style="15" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="14"/>
+    <col min="20" max="20" width="11.5703125" style="15" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" style="14" customWidth="1"/>
+    <col min="22" max="25" width="9.140625" style="14"/>
     <col min="30" max="30" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:33" s="27" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="S1" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="T1" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="22" t="s">
+      <c r="U1" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="V1" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="W1" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="4"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="8"/>
+      <c r="AD1" s="28"/>
       <c r="AE1" s="5"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
       <c r="Z2" s="6"/>
       <c r="AE2" s="7"/>
       <c r="AF2" s="6"/>
       <c r="AG2" s="6"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
+      <c r="C3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
       <c r="Z3" s="6"/>
       <c r="AE3" s="7"/>
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
       <c r="Z4" s="6"/>
       <c r="AE4" s="7"/>
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
+      <c r="C5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
       <c r="Z5" s="6"/>
       <c r="AE5" s="7"/>
       <c r="AF5" s="6"/>
       <c r="AG5" s="6"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
       <c r="Z6" s="6"/>
       <c r="AE6" s="7"/>
       <c r="AF6" s="6"/>
       <c r="AG6" s="6"/>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
+      <c r="C7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
       <c r="Z7" s="6"/>
       <c r="AE7" s="7"/>
       <c r="AF7" s="6"/>
       <c r="AG7" s="6"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
       <c r="Z8" s="6"/>
       <c r="AE8" s="7"/>
       <c r="AF8" s="6"/>
       <c r="AG8" s="6"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
+      <c r="C9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
       <c r="Z9" s="6"/>
       <c r="AE9" s="7"/>
       <c r="AF9" s="6"/>
       <c r="AG9" s="6"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
       <c r="Z10" s="6"/>
       <c r="AE10" s="6"/>
       <c r="AF10" s="6"/>
       <c r="AG10" s="6"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
+      <c r="C11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
       <c r="Z11" s="6"/>
       <c r="AE11" s="6"/>
       <c r="AF11" s="6"/>
       <c r="AG11" s="6"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
       <c r="Z12" s="6"/>
       <c r="AE12" s="6"/>
       <c r="AF12" s="6"/>
       <c r="AG12" s="6"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+      <c r="C13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
       <c r="Z13" s="6"/>
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
@@ -2975,17 +2998,17 @@
       <c r="AG13" s="6"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
       <c r="Z14" s="6"/>
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
@@ -2996,15 +3019,15 @@
       <c r="AG14" s="6"/>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
+      <c r="C15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
       <c r="Z15" s="6"/>
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
@@ -3015,17 +3038,17 @@
       <c r="AG15" s="6"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
       <c r="Z16" s="6"/>
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
@@ -3036,15 +3059,15 @@
       <c r="AG16" s="6"/>
     </row>
     <row r="17" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="C17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
+      <c r="C17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
       <c r="Z17" s="6"/>
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
@@ -3055,856 +3078,856 @@
       <c r="AG17" s="6"/>
     </row>
     <row r="18" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
     </row>
     <row r="19" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
     </row>
     <row r="20" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
     </row>
     <row r="21" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
     </row>
     <row r="22" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
     </row>
     <row r="23" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
     </row>
     <row r="24" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
     </row>
     <row r="25" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
     </row>
     <row r="26" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
     </row>
     <row r="27" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
     </row>
     <row r="28" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
     </row>
     <row r="29" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
     </row>
     <row r="30" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
     </row>
     <row r="31" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
     </row>
     <row r="32" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
     </row>
     <row r="33" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N33" s="14"/>
+      <c r="N33" s="13"/>
     </row>
     <row r="34" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N34" s="14"/>
+      <c r="N34" s="13"/>
     </row>
     <row r="35" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N35" s="14"/>
+      <c r="N35" s="13"/>
     </row>
     <row r="36" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N36" s="14"/>
+      <c r="N36" s="13"/>
     </row>
     <row r="37" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N37" s="14"/>
+      <c r="N37" s="13"/>
     </row>
     <row r="38" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N38" s="14"/>
+      <c r="N38" s="13"/>
     </row>
     <row r="39" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N39" s="14"/>
-      <c r="P39" s="14"/>
+      <c r="N39" s="13"/>
+      <c r="P39" s="13"/>
     </row>
     <row r="40" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N40" s="14"/>
-      <c r="P40" s="14"/>
+      <c r="N40" s="13"/>
+      <c r="P40" s="13"/>
     </row>
     <row r="41" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N41" s="14"/>
-      <c r="P41" s="14"/>
+      <c r="N41" s="13"/>
+      <c r="P41" s="13"/>
     </row>
     <row r="42" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N42" s="14"/>
-      <c r="P42" s="14"/>
+      <c r="N42" s="13"/>
+      <c r="P42" s="13"/>
     </row>
     <row r="43" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N43" s="14"/>
-      <c r="P43" s="14"/>
+      <c r="N43" s="13"/>
+      <c r="P43" s="13"/>
     </row>
     <row r="44" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N44" s="14"/>
-      <c r="P44" s="14"/>
+      <c r="N44" s="13"/>
+      <c r="P44" s="13"/>
     </row>
     <row r="45" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N45" s="14"/>
-      <c r="P45" s="14"/>
+      <c r="N45" s="13"/>
+      <c r="P45" s="13"/>
     </row>
     <row r="46" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N46" s="14"/>
-      <c r="P46" s="14"/>
+      <c r="N46" s="13"/>
+      <c r="P46" s="13"/>
     </row>
     <row r="47" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N47" s="14"/>
-      <c r="P47" s="14"/>
+      <c r="N47" s="13"/>
+      <c r="P47" s="13"/>
     </row>
     <row r="48" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N48" s="14"/>
-      <c r="P48" s="14"/>
+      <c r="N48" s="13"/>
+      <c r="P48" s="13"/>
     </row>
     <row r="49" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N49" s="14"/>
-      <c r="P49" s="14"/>
+      <c r="N49" s="13"/>
+      <c r="P49" s="13"/>
     </row>
     <row r="50" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N50" s="14"/>
-      <c r="P50" s="14"/>
+      <c r="N50" s="13"/>
+      <c r="P50" s="13"/>
     </row>
     <row r="51" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N51" s="14"/>
-      <c r="P51" s="14"/>
+      <c r="N51" s="13"/>
+      <c r="P51" s="13"/>
     </row>
     <row r="52" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N52" s="14"/>
-      <c r="P52" s="14"/>
+      <c r="N52" s="13"/>
+      <c r="P52" s="13"/>
     </row>
     <row r="53" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N53" s="14"/>
-      <c r="P53" s="14"/>
+      <c r="N53" s="13"/>
+      <c r="P53" s="13"/>
     </row>
     <row r="54" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N54" s="14"/>
-      <c r="P54" s="14"/>
+      <c r="N54" s="13"/>
+      <c r="P54" s="13"/>
     </row>
     <row r="55" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N55" s="14"/>
-      <c r="P55" s="14"/>
+      <c r="N55" s="13"/>
+      <c r="P55" s="13"/>
     </row>
     <row r="56" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N56" s="14"/>
-      <c r="P56" s="14"/>
+      <c r="N56" s="13"/>
+      <c r="P56" s="13"/>
     </row>
     <row r="57" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N57" s="14"/>
-      <c r="P57" s="14"/>
+      <c r="N57" s="13"/>
+      <c r="P57" s="13"/>
     </row>
     <row r="58" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N58" s="14"/>
-      <c r="P58" s="14"/>
+      <c r="N58" s="13"/>
+      <c r="P58" s="13"/>
     </row>
     <row r="59" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N59" s="14"/>
-      <c r="P59" s="14"/>
+      <c r="N59" s="13"/>
+      <c r="P59" s="13"/>
     </row>
     <row r="60" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N60" s="14"/>
-      <c r="P60" s="14"/>
+      <c r="N60" s="13"/>
+      <c r="P60" s="13"/>
     </row>
     <row r="61" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N61" s="14"/>
-      <c r="P61" s="14"/>
+      <c r="N61" s="13"/>
+      <c r="P61" s="13"/>
     </row>
     <row r="62" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N62" s="14"/>
-      <c r="P62" s="14"/>
+      <c r="N62" s="13"/>
+      <c r="P62" s="13"/>
     </row>
     <row r="63" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N63" s="14"/>
-      <c r="P63" s="14"/>
+      <c r="N63" s="13"/>
+      <c r="P63" s="13"/>
     </row>
     <row r="64" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N64" s="14"/>
-      <c r="P64" s="14"/>
+      <c r="N64" s="13"/>
+      <c r="P64" s="13"/>
     </row>
     <row r="65" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N65" s="14"/>
-      <c r="P65" s="14"/>
+      <c r="N65" s="13"/>
+      <c r="P65" s="13"/>
     </row>
     <row r="66" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N66" s="14"/>
-      <c r="P66" s="14"/>
+      <c r="N66" s="13"/>
+      <c r="P66" s="13"/>
     </row>
     <row r="67" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N67" s="14"/>
-      <c r="P67" s="14"/>
+      <c r="N67" s="13"/>
+      <c r="P67" s="13"/>
     </row>
     <row r="68" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N68" s="14"/>
-      <c r="P68" s="14"/>
+      <c r="N68" s="13"/>
+      <c r="P68" s="13"/>
     </row>
     <row r="69" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N69" s="14"/>
-      <c r="P69" s="14"/>
+      <c r="N69" s="13"/>
+      <c r="P69" s="13"/>
     </row>
     <row r="70" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N70" s="14"/>
-      <c r="P70" s="14"/>
+      <c r="N70" s="13"/>
+      <c r="P70" s="13"/>
     </row>
     <row r="71" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N71" s="14"/>
-      <c r="P71" s="14"/>
+      <c r="N71" s="13"/>
+      <c r="P71" s="13"/>
     </row>
     <row r="72" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N72" s="14"/>
-      <c r="P72" s="14"/>
+      <c r="N72" s="13"/>
+      <c r="P72" s="13"/>
     </row>
     <row r="73" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N73" s="14"/>
-      <c r="P73" s="14"/>
+      <c r="N73" s="13"/>
+      <c r="P73" s="13"/>
     </row>
     <row r="74" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N74" s="14"/>
-      <c r="P74" s="14"/>
+      <c r="N74" s="13"/>
+      <c r="P74" s="13"/>
     </row>
     <row r="75" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N75" s="14"/>
-      <c r="P75" s="14"/>
+      <c r="N75" s="13"/>
+      <c r="P75" s="13"/>
     </row>
     <row r="76" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N76" s="14"/>
-      <c r="P76" s="14"/>
+      <c r="N76" s="13"/>
+      <c r="P76" s="13"/>
     </row>
     <row r="77" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N77" s="14"/>
-      <c r="P77" s="14"/>
+      <c r="N77" s="13"/>
+      <c r="P77" s="13"/>
     </row>
     <row r="78" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N78" s="14"/>
-      <c r="P78" s="14"/>
+      <c r="N78" s="13"/>
+      <c r="P78" s="13"/>
     </row>
     <row r="79" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N79" s="14"/>
-      <c r="P79" s="14"/>
+      <c r="N79" s="13"/>
+      <c r="P79" s="13"/>
     </row>
     <row r="80" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N80" s="14"/>
-      <c r="P80" s="14"/>
+      <c r="N80" s="13"/>
+      <c r="P80" s="13"/>
     </row>
     <row r="81" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N81" s="14"/>
-      <c r="P81" s="14"/>
+      <c r="N81" s="13"/>
+      <c r="P81" s="13"/>
     </row>
     <row r="82" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N82" s="14"/>
-      <c r="P82" s="14"/>
+      <c r="N82" s="13"/>
+      <c r="P82" s="13"/>
     </row>
     <row r="83" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N83" s="14"/>
-      <c r="P83" s="14"/>
+      <c r="N83" s="13"/>
+      <c r="P83" s="13"/>
     </row>
     <row r="84" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N84" s="14"/>
-      <c r="P84" s="14"/>
+      <c r="N84" s="13"/>
+      <c r="P84" s="13"/>
     </row>
     <row r="85" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N85" s="14"/>
-      <c r="P85" s="14"/>
+      <c r="N85" s="13"/>
+      <c r="P85" s="13"/>
     </row>
     <row r="86" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N86" s="14"/>
-      <c r="P86" s="14"/>
+      <c r="N86" s="13"/>
+      <c r="P86" s="13"/>
     </row>
     <row r="87" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N87" s="14"/>
-      <c r="P87" s="14"/>
+      <c r="N87" s="13"/>
+      <c r="P87" s="13"/>
     </row>
     <row r="88" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N88" s="14"/>
-      <c r="P88" s="14"/>
+      <c r="N88" s="13"/>
+      <c r="P88" s="13"/>
     </row>
     <row r="89" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N89" s="14"/>
-      <c r="P89" s="14"/>
+      <c r="N89" s="13"/>
+      <c r="P89" s="13"/>
     </row>
     <row r="90" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N90" s="14"/>
-      <c r="P90" s="14"/>
+      <c r="N90" s="13"/>
+      <c r="P90" s="13"/>
     </row>
     <row r="91" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N91" s="14"/>
-      <c r="P91" s="14"/>
+      <c r="N91" s="13"/>
+      <c r="P91" s="13"/>
     </row>
     <row r="92" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N92" s="14"/>
-      <c r="P92" s="14"/>
+      <c r="N92" s="13"/>
+      <c r="P92" s="13"/>
     </row>
     <row r="93" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N93" s="14"/>
-      <c r="P93" s="14"/>
+      <c r="N93" s="13"/>
+      <c r="P93" s="13"/>
     </row>
     <row r="94" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N94" s="14"/>
-      <c r="P94" s="14"/>
+      <c r="N94" s="13"/>
+      <c r="P94" s="13"/>
     </row>
     <row r="95" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N95" s="14"/>
-      <c r="P95" s="14"/>
+      <c r="N95" s="13"/>
+      <c r="P95" s="13"/>
     </row>
     <row r="96" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N96" s="14"/>
-      <c r="P96" s="14"/>
+      <c r="N96" s="13"/>
+      <c r="P96" s="13"/>
     </row>
     <row r="97" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N97" s="14"/>
-      <c r="P97" s="14"/>
+      <c r="N97" s="13"/>
+      <c r="P97" s="13"/>
     </row>
     <row r="98" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N98" s="14"/>
-      <c r="P98" s="14"/>
+      <c r="N98" s="13"/>
+      <c r="P98" s="13"/>
     </row>
     <row r="99" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N99" s="14"/>
-      <c r="P99" s="14"/>
+      <c r="N99" s="13"/>
+      <c r="P99" s="13"/>
     </row>
     <row r="100" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N100" s="14"/>
-      <c r="P100" s="14"/>
+      <c r="N100" s="13"/>
+      <c r="P100" s="13"/>
     </row>
     <row r="101" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N101" s="14"/>
-      <c r="P101" s="14"/>
+      <c r="N101" s="13"/>
+      <c r="P101" s="13"/>
     </row>
     <row r="102" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N102" s="14"/>
-      <c r="P102" s="14"/>
+      <c r="N102" s="13"/>
+      <c r="P102" s="13"/>
     </row>
     <row r="103" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N103" s="14"/>
-      <c r="P103" s="14"/>
+      <c r="N103" s="13"/>
+      <c r="P103" s="13"/>
     </row>
     <row r="104" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N104" s="14"/>
-      <c r="P104" s="14"/>
+      <c r="N104" s="13"/>
+      <c r="P104" s="13"/>
     </row>
     <row r="105" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N105" s="14"/>
-      <c r="P105" s="14"/>
+      <c r="N105" s="13"/>
+      <c r="P105" s="13"/>
     </row>
     <row r="106" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N106" s="14"/>
-      <c r="P106" s="14"/>
+      <c r="N106" s="13"/>
+      <c r="P106" s="13"/>
     </row>
     <row r="107" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N107" s="14"/>
-      <c r="P107" s="14"/>
+      <c r="N107" s="13"/>
+      <c r="P107" s="13"/>
     </row>
     <row r="108" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N108" s="14"/>
-      <c r="P108" s="14"/>
+      <c r="N108" s="13"/>
+      <c r="P108" s="13"/>
     </row>
     <row r="109" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N109" s="14"/>
-      <c r="P109" s="14"/>
+      <c r="N109" s="13"/>
+      <c r="P109" s="13"/>
     </row>
     <row r="110" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N110" s="14"/>
-      <c r="P110" s="14"/>
+      <c r="N110" s="13"/>
+      <c r="P110" s="13"/>
     </row>
     <row r="111" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N111" s="14"/>
-      <c r="P111" s="14"/>
+      <c r="N111" s="13"/>
+      <c r="P111" s="13"/>
     </row>
     <row r="112" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N112" s="14"/>
-      <c r="P112" s="14"/>
+      <c r="N112" s="13"/>
+      <c r="P112" s="13"/>
     </row>
     <row r="113" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N113" s="14"/>
-      <c r="P113" s="14"/>
+      <c r="N113" s="13"/>
+      <c r="P113" s="13"/>
     </row>
     <row r="114" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N114" s="14"/>
-      <c r="P114" s="14"/>
+      <c r="N114" s="13"/>
+      <c r="P114" s="13"/>
     </row>
     <row r="115" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N115" s="14"/>
-      <c r="P115" s="14"/>
+      <c r="N115" s="13"/>
+      <c r="P115" s="13"/>
     </row>
     <row r="116" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N116" s="14"/>
-      <c r="P116" s="14"/>
+      <c r="N116" s="13"/>
+      <c r="P116" s="13"/>
     </row>
     <row r="117" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N117" s="14"/>
-      <c r="P117" s="14"/>
+      <c r="N117" s="13"/>
+      <c r="P117" s="13"/>
     </row>
     <row r="118" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N118" s="14"/>
-      <c r="P118" s="14"/>
+      <c r="N118" s="13"/>
+      <c r="P118" s="13"/>
     </row>
     <row r="119" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N119" s="14"/>
-      <c r="P119" s="14"/>
+      <c r="N119" s="13"/>
+      <c r="P119" s="13"/>
     </row>
     <row r="120" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N120" s="14"/>
-      <c r="P120" s="14"/>
+      <c r="N120" s="13"/>
+      <c r="P120" s="13"/>
     </row>
     <row r="121" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N121" s="14"/>
-      <c r="P121" s="14"/>
+      <c r="N121" s="13"/>
+      <c r="P121" s="13"/>
     </row>
     <row r="122" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N122" s="14"/>
-      <c r="P122" s="14"/>
+      <c r="N122" s="13"/>
+      <c r="P122" s="13"/>
     </row>
     <row r="123" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N123" s="14"/>
-      <c r="P123" s="14"/>
+      <c r="N123" s="13"/>
+      <c r="P123" s="13"/>
     </row>
     <row r="124" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N124" s="14"/>
-      <c r="P124" s="14"/>
+      <c r="N124" s="13"/>
+      <c r="P124" s="13"/>
     </row>
     <row r="125" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N125" s="14"/>
-      <c r="P125" s="14"/>
+      <c r="N125" s="13"/>
+      <c r="P125" s="13"/>
     </row>
     <row r="126" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N126" s="14"/>
-      <c r="P126" s="14"/>
+      <c r="N126" s="13"/>
+      <c r="P126" s="13"/>
     </row>
     <row r="127" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N127" s="14"/>
-      <c r="P127" s="14"/>
+      <c r="N127" s="13"/>
+      <c r="P127" s="13"/>
     </row>
     <row r="128" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N128" s="14"/>
-      <c r="P128" s="14"/>
+      <c r="N128" s="13"/>
+      <c r="P128" s="13"/>
     </row>
     <row r="129" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N129" s="14"/>
-      <c r="P129" s="14"/>
+      <c r="N129" s="13"/>
+      <c r="P129" s="13"/>
     </row>
     <row r="130" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N130" s="14"/>
-      <c r="P130" s="14"/>
+      <c r="N130" s="13"/>
+      <c r="P130" s="13"/>
     </row>
     <row r="131" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N131" s="14"/>
-      <c r="P131" s="14"/>
+      <c r="N131" s="13"/>
+      <c r="P131" s="13"/>
     </row>
     <row r="132" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N132" s="14"/>
-      <c r="P132" s="14"/>
+      <c r="N132" s="13"/>
+      <c r="P132" s="13"/>
     </row>
     <row r="133" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N133" s="14"/>
-      <c r="P133" s="14"/>
+      <c r="N133" s="13"/>
+      <c r="P133" s="13"/>
     </row>
     <row r="134" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N134" s="14"/>
-      <c r="P134" s="14"/>
+      <c r="N134" s="13"/>
+      <c r="P134" s="13"/>
     </row>
     <row r="135" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N135" s="14"/>
-      <c r="P135" s="14"/>
+      <c r="N135" s="13"/>
+      <c r="P135" s="13"/>
     </row>
     <row r="136" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N136" s="14"/>
-      <c r="P136" s="14"/>
+      <c r="N136" s="13"/>
+      <c r="P136" s="13"/>
     </row>
     <row r="137" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N137" s="14"/>
-      <c r="P137" s="14"/>
+      <c r="N137" s="13"/>
+      <c r="P137" s="13"/>
     </row>
     <row r="138" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N138" s="14"/>
-      <c r="P138" s="14"/>
+      <c r="N138" s="13"/>
+      <c r="P138" s="13"/>
     </row>
     <row r="139" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N139" s="14"/>
-      <c r="P139" s="14"/>
+      <c r="N139" s="13"/>
+      <c r="P139" s="13"/>
     </row>
     <row r="140" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N140" s="14"/>
-      <c r="P140" s="14"/>
+      <c r="N140" s="13"/>
+      <c r="P140" s="13"/>
     </row>
     <row r="141" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N141" s="14"/>
-      <c r="P141" s="14"/>
+      <c r="N141" s="13"/>
+      <c r="P141" s="13"/>
     </row>
     <row r="142" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N142" s="14"/>
-      <c r="P142" s="14"/>
+      <c r="N142" s="13"/>
+      <c r="P142" s="13"/>
     </row>
     <row r="143" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N143" s="14"/>
-      <c r="P143" s="14"/>
+      <c r="N143" s="13"/>
+      <c r="P143" s="13"/>
     </row>
     <row r="144" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N144" s="14"/>
-      <c r="P144" s="14"/>
+      <c r="N144" s="13"/>
+      <c r="P144" s="13"/>
     </row>
     <row r="145" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N145" s="14"/>
-      <c r="P145" s="14"/>
+      <c r="N145" s="13"/>
+      <c r="P145" s="13"/>
     </row>
     <row r="146" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N146" s="14"/>
-      <c r="P146" s="14"/>
+      <c r="N146" s="13"/>
+      <c r="P146" s="13"/>
     </row>
     <row r="147" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N147" s="14"/>
-      <c r="P147" s="14"/>
+      <c r="N147" s="13"/>
+      <c r="P147" s="13"/>
     </row>
     <row r="148" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N148" s="14"/>
-      <c r="P148" s="14"/>
+      <c r="N148" s="13"/>
+      <c r="P148" s="13"/>
     </row>
     <row r="149" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N149" s="14"/>
-      <c r="P149" s="14"/>
+      <c r="N149" s="13"/>
+      <c r="P149" s="13"/>
     </row>
     <row r="150" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N150" s="14"/>
-      <c r="P150" s="14"/>
+      <c r="N150" s="13"/>
+      <c r="P150" s="13"/>
     </row>
     <row r="151" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N151" s="14"/>
-      <c r="P151" s="14"/>
+      <c r="N151" s="13"/>
+      <c r="P151" s="13"/>
     </row>
     <row r="152" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N152" s="14"/>
-      <c r="P152" s="14"/>
+      <c r="N152" s="13"/>
+      <c r="P152" s="13"/>
     </row>
     <row r="153" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N153" s="14"/>
-      <c r="P153" s="14"/>
+      <c r="N153" s="13"/>
+      <c r="P153" s="13"/>
     </row>
     <row r="154" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N154" s="14"/>
-      <c r="P154" s="14"/>
+      <c r="N154" s="13"/>
+      <c r="P154" s="13"/>
     </row>
     <row r="155" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N155" s="14"/>
-      <c r="P155" s="14"/>
+      <c r="N155" s="13"/>
+      <c r="P155" s="13"/>
     </row>
     <row r="156" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="P156" s="14"/>
+      <c r="P156" s="13"/>
     </row>
     <row r="157" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="P157" s="14"/>
+      <c r="P157" s="13"/>
     </row>
     <row r="158" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="P158" s="14"/>
+      <c r="P158" s="13"/>
     </row>
     <row r="159" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="P159" s="14"/>
+      <c r="P159" s="13"/>
     </row>
     <row r="160" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="P160" s="14"/>
+      <c r="P160" s="13"/>
     </row>
     <row r="161" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P161" s="14"/>
+      <c r="P161" s="13"/>
     </row>
     <row r="162" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P162" s="14"/>
+      <c r="P162" s="13"/>
     </row>
     <row r="163" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P163" s="14"/>
+      <c r="P163" s="13"/>
     </row>
     <row r="164" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P164" s="14"/>
+      <c r="P164" s="13"/>
     </row>
     <row r="165" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P165" s="14"/>
+      <c r="P165" s="13"/>
     </row>
     <row r="166" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P166" s="14"/>
+      <c r="P166" s="13"/>
     </row>
     <row r="167" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P167" s="14"/>
+      <c r="P167" s="13"/>
     </row>
     <row r="168" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P168" s="14"/>
+      <c r="P168" s="13"/>
     </row>
     <row r="169" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P169" s="14"/>
+      <c r="P169" s="13"/>
     </row>
     <row r="170" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P170" s="14"/>
+      <c r="P170" s="13"/>
     </row>
     <row r="171" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P171" s="14"/>
+      <c r="P171" s="13"/>
     </row>
     <row r="172" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P172" s="14"/>
+      <c r="P172" s="13"/>
     </row>
     <row r="173" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P173" s="14"/>
+      <c r="P173" s="13"/>
     </row>
     <row r="174" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P174" s="14"/>
+      <c r="P174" s="13"/>
     </row>
     <row r="175" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P175" s="14"/>
+      <c r="P175" s="13"/>
     </row>
     <row r="176" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P176" s="14"/>
+      <c r="P176" s="13"/>
     </row>
     <row r="177" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P177" s="14"/>
+      <c r="P177" s="13"/>
     </row>
     <row r="178" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P178" s="14"/>
+      <c r="P178" s="13"/>
     </row>
     <row r="179" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P179" s="14"/>
+      <c r="P179" s="13"/>
     </row>
     <row r="180" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P180" s="14"/>
+      <c r="P180" s="13"/>
     </row>
     <row r="181" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P181" s="14"/>
+      <c r="P181" s="13"/>
     </row>
     <row r="182" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P182" s="14"/>
+      <c r="P182" s="13"/>
     </row>
     <row r="183" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P183" s="14"/>
+      <c r="P183" s="13"/>
     </row>
     <row r="184" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P184" s="14"/>
+      <c r="P184" s="13"/>
     </row>
     <row r="185" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P185" s="14"/>
+      <c r="P185" s="13"/>
     </row>
     <row r="186" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P186" s="14"/>
+      <c r="P186" s="13"/>
     </row>
     <row r="187" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P187" s="14"/>
+      <c r="P187" s="13"/>
     </row>
     <row r="188" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P188" s="14"/>
+      <c r="P188" s="13"/>
     </row>
     <row r="189" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P189" s="14"/>
+      <c r="P189" s="13"/>
     </row>
     <row r="190" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P190" s="14"/>
+      <c r="P190" s="13"/>
     </row>
     <row r="191" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P191" s="14"/>
+      <c r="P191" s="13"/>
     </row>
     <row r="192" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P192" s="14"/>
+      <c r="P192" s="13"/>
     </row>
     <row r="193" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P193" s="14"/>
+      <c r="P193" s="13"/>
     </row>
     <row r="194" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P194" s="14"/>
+      <c r="P194" s="13"/>
     </row>
     <row r="195" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P195" s="14"/>
+      <c r="P195" s="13"/>
     </row>
     <row r="196" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P196" s="14"/>
+      <c r="P196" s="13"/>
     </row>
     <row r="197" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P197" s="14"/>
+      <c r="P197" s="13"/>
     </row>
     <row r="198" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P198" s="14"/>
+      <c r="P198" s="13"/>
     </row>
     <row r="199" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P199" s="14"/>
+      <c r="P199" s="13"/>
     </row>
     <row r="200" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P200" s="14"/>
+      <c r="P200" s="13"/>
     </row>
     <row r="201" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P201" s="14"/>
+      <c r="P201" s="13"/>
     </row>
     <row r="202" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P202" s="14"/>
+      <c r="P202" s="13"/>
     </row>
     <row r="203" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P203" s="14"/>
+      <c r="P203" s="13"/>
     </row>
     <row r="204" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P204" s="14"/>
+      <c r="P204" s="13"/>
     </row>
     <row r="205" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P205" s="14"/>
+      <c r="P205" s="13"/>
     </row>
     <row r="206" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P206" s="14"/>
+      <c r="P206" s="13"/>
     </row>
     <row r="207" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P207" s="14"/>
+      <c r="P207" s="13"/>
     </row>
     <row r="208" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P208" s="14"/>
+      <c r="P208" s="13"/>
     </row>
     <row r="209" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P209" s="14"/>
+      <c r="P209" s="13"/>
     </row>
     <row r="210" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P210" s="14"/>
+      <c r="P210" s="13"/>
     </row>
     <row r="211" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P211" s="14"/>
+      <c r="P211" s="13"/>
     </row>
     <row r="212" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P212" s="14"/>
+      <c r="P212" s="13"/>
     </row>
     <row r="213" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P213" s="14"/>
+      <c r="P213" s="13"/>
     </row>
     <row r="214" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P214" s="14"/>
+      <c r="P214" s="13"/>
     </row>
     <row r="215" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P215" s="14"/>
+      <c r="P215" s="13"/>
     </row>
     <row r="216" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P216" s="14"/>
+      <c r="P216" s="13"/>
     </row>
     <row r="217" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P217" s="14"/>
+      <c r="P217" s="13"/>
     </row>
     <row r="218" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P218" s="14"/>
+      <c r="P218" s="13"/>
     </row>
     <row r="219" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P219" s="14"/>
+      <c r="P219" s="13"/>
     </row>
     <row r="220" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P220" s="14"/>
+      <c r="P220" s="13"/>
     </row>
     <row r="221" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P221" s="14"/>
+      <c r="P221" s="13"/>
     </row>
     <row r="222" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P222" s="14"/>
+      <c r="P222" s="13"/>
     </row>
     <row r="223" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P223" s="14"/>
+      <c r="P223" s="13"/>
     </row>
     <row r="224" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P224" s="14"/>
+      <c r="P224" s="13"/>
     </row>
     <row r="225" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P225" s="14"/>
+      <c r="P225" s="13"/>
     </row>
     <row r="226" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P226" s="14"/>
+      <c r="P226" s="13"/>
     </row>
     <row r="227" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P227" s="14"/>
+      <c r="P227" s="13"/>
     </row>
     <row r="228" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P228" s="14"/>
+      <c r="P228" s="13"/>
     </row>
     <row r="229" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P229" s="14"/>
+      <c r="P229" s="13"/>
     </row>
     <row r="230" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P230" s="14"/>
+      <c r="P230" s="13"/>
     </row>
     <row r="231" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P231" s="14"/>
+      <c r="P231" s="13"/>
     </row>
     <row r="232" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P232" s="14"/>
+      <c r="P232" s="13"/>
     </row>
     <row r="233" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P233" s="14"/>
+      <c r="P233" s="13"/>
     </row>
     <row r="234" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P234" s="14"/>
+      <c r="P234" s="13"/>
     </row>
     <row r="235" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P235" s="14"/>
+      <c r="P235" s="13"/>
     </row>
     <row r="236" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P236" s="14"/>
+      <c r="P236" s="13"/>
     </row>
     <row r="237" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P237" s="14"/>
+      <c r="P237" s="13"/>
     </row>
     <row r="238" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P238" s="14"/>
+      <c r="P238" s="13"/>
     </row>
     <row r="239" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P239" s="14"/>
+      <c r="P239" s="13"/>
     </row>
     <row r="240" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P240" s="14"/>
+      <c r="P240" s="13"/>
     </row>
     <row r="241" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P241" s="14"/>
+      <c r="P241" s="13"/>
     </row>
     <row r="242" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P242" s="14"/>
+      <c r="P242" s="13"/>
     </row>
     <row r="243" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P243" s="14"/>
+      <c r="P243" s="13"/>
     </row>
     <row r="244" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P244" s="14"/>
+      <c r="P244" s="13"/>
     </row>
     <row r="245" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P245" s="14"/>
+      <c r="P245" s="13"/>
     </row>
     <row r="246" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P246" s="14"/>
+      <c r="P246" s="13"/>
     </row>
     <row r="247" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P247" s="14"/>
+      <c r="P247" s="13"/>
     </row>
     <row r="248" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P248" s="14"/>
+      <c r="P248" s="13"/>
     </row>
     <row r="249" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P249" s="14"/>
+      <c r="P249" s="13"/>
     </row>
     <row r="250" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P250" s="14"/>
+      <c r="P250" s="13"/>
     </row>
     <row r="251" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P251" s="14"/>
+      <c r="P251" s="13"/>
     </row>
     <row r="252" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P252" s="14"/>
+      <c r="P252" s="13"/>
     </row>
     <row r="253" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P253" s="14"/>
+      <c r="P253" s="13"/>
     </row>
     <row r="254" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P254" s="14"/>
+      <c r="P254" s="13"/>
     </row>
     <row r="255" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P255" s="14"/>
+      <c r="P255" s="13"/>
     </row>
     <row r="256" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P256" s="14"/>
+      <c r="P256" s="13"/>
     </row>
     <row r="257" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P257" s="14"/>
+      <c r="P257" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3962,7 +3985,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$D$3:$D$12</xm:f>
           </x14:formula1>
-          <xm:sqref>I1:I1048576</xm:sqref>
+          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3995,25 +4018,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>10</v>
+      <c r="G1" s="11" t="s">
+        <v>4</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -4024,248 +4047,248 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="H5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="G9" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>